<commit_message>
Updates to support worker init/final scripts in 2.x world.
</commit_message>
<xml_diff>
--- a/spec/files/0_3_7_worker_init_final.xlsx
+++ b/spec/files/0_3_7_worker_init_final.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19840" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -2566,9 +2566,6 @@
     <t>["first_arg",2,{a_hash: "input"}]</t>
   </si>
   <si>
-    <t>../../spec/files/worker_init/second_file.rb</t>
-  </si>
-  <si>
     <t>do something else</t>
   </si>
   <si>
@@ -2588,6 +2585,9 @@
   </si>
   <si>
     <t>0_3_7_worker_init_final</t>
+  </si>
+  <si>
+    <t>../../spec/files/worker_init/second_file.sh</t>
   </si>
 </sst>
 </file>
@@ -6791,7 +6791,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6804,7 +6803,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -6965,7 +6966,7 @@
         <v>40</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>470</v>
@@ -7318,7 +7319,7 @@
       </c>
       <c r="D46" s="25"/>
       <c r="E46" s="13" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -7334,25 +7335,25 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="29" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>841</v>
+        <v>848</v>
       </c>
       <c r="C48" s="29"/>
     </row>
     <row r="49" spans="1:5" s="29" customFormat="1">
       <c r="B49" s="24" t="s">
-        <v>841</v>
+        <v>848</v>
       </c>
       <c r="C49" s="29" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D49" s="2"/>
     </row>
     <row r="51" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A51" s="11" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B51" s="25" t="s">
         <v>835</v>
@@ -7362,7 +7363,7 @@
       </c>
       <c r="D51" s="25"/>
       <c r="E51" s="13" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -7373,7 +7374,7 @@
         <v>839</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
   </sheetData>
@@ -7392,7 +7393,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7993,7 +7993,6 @@
     <mergeCell ref="U1:Z1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -10656,7 +10655,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -18826,7 +18824,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -19321,7 +19318,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>